<commit_message>
Added incorrect email and password case
</commit_message>
<xml_diff>
--- a/RPAFramework/RoboticEnterpriseFramework/Data/Config.xlsx
+++ b/RPAFramework/RoboticEnterpriseFramework/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\RPA\RPAFramework\RoboticEnterpriseFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\RPA\RPAProiect\YoutubePlaylistCreator\RPAFramework\RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CD15C-F6B2-4F4F-B263-88AF99AF04B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1643BE8A-14BE-4395-AC03-8A20005FB857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>www.youtube.com</t>
+  </si>
+  <si>
+    <t>RetryNumberYoutubeDown</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -591,7 +594,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>